<commit_message>
Refresh range search diagram
</commit_message>
<xml_diff>
--- a/docs/report.xlsx
+++ b/docs/report.xlsx
@@ -685,7 +685,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1290,9 +1289,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000002-B19A-42FB-A80C-789D11B63562}"/>
                 </c:ext>
@@ -1314,9 +1311,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000003-B19A-42FB-A80C-789D11B63562}"/>
                 </c:ext>
@@ -1338,9 +1333,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000004-B19A-42FB-A80C-789D11B63562}"/>
                 </c:ext>
@@ -1362,9 +1355,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000005-B19A-42FB-A80C-789D11B63562}"/>
                 </c:ext>
@@ -1386,9 +1377,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{0000000A-B19A-42FB-A80C-789D11B63562}"/>
                 </c:ext>
@@ -1420,9 +1409,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000008-B19A-42FB-A80C-789D11B63562}"/>
                 </c:ext>
@@ -1444,9 +1431,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000007-B19A-42FB-A80C-789D11B63562}"/>
                 </c:ext>
@@ -1468,9 +1453,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000006-B19A-42FB-A80C-789D11B63562}"/>
                 </c:ext>
@@ -1515,7 +1498,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1680,9 +1662,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{0000000B-B19A-42FB-A80C-789D11B63562}"/>
                 </c:ext>
@@ -1704,9 +1684,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{0000000C-B19A-42FB-A80C-789D11B63562}"/>
                 </c:ext>
@@ -1728,9 +1706,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{0000000D-B19A-42FB-A80C-789D11B63562}"/>
                 </c:ext>
@@ -1752,9 +1728,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{0000000E-B19A-42FB-A80C-789D11B63562}"/>
                 </c:ext>
@@ -1786,9 +1760,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000011-B19A-42FB-A80C-789D11B63562}"/>
                 </c:ext>
@@ -1810,9 +1782,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000010-B19A-42FB-A80C-789D11B63562}"/>
                 </c:ext>
@@ -1834,9 +1804,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000012-B19A-42FB-A80C-789D11B63562}"/>
                 </c:ext>
@@ -1858,9 +1826,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000013-B19A-42FB-A80C-789D11B63562}"/>
                 </c:ext>
@@ -1882,9 +1848,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000014-B19A-42FB-A80C-789D11B63562}"/>
                 </c:ext>
@@ -1906,9 +1870,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000015-B19A-42FB-A80C-789D11B63562}"/>
                 </c:ext>
@@ -1953,7 +1915,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2208,7 +2169,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2340,7 +2300,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2552,7 +2511,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3157,9 +3115,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000004-CF2F-4B92-BF82-37AF6163439F}"/>
                 </c:ext>
@@ -3181,9 +3137,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000005-CF2F-4B92-BF82-37AF6163439F}"/>
                 </c:ext>
@@ -3205,9 +3159,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000006-CF2F-4B92-BF82-37AF6163439F}"/>
                 </c:ext>
@@ -3229,9 +3181,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000007-CF2F-4B92-BF82-37AF6163439F}"/>
                 </c:ext>
@@ -3253,9 +3203,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000008-CF2F-4B92-BF82-37AF6163439F}"/>
                 </c:ext>
@@ -3287,9 +3235,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{0000000A-CF2F-4B92-BF82-37AF6163439F}"/>
                 </c:ext>
@@ -3311,9 +3257,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{0000000B-CF2F-4B92-BF82-37AF6163439F}"/>
                 </c:ext>
@@ -3335,9 +3279,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{0000000C-CF2F-4B92-BF82-37AF6163439F}"/>
                 </c:ext>
@@ -3382,7 +3324,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -3547,9 +3488,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{0000000E-CF2F-4B92-BF82-37AF6163439F}"/>
                 </c:ext>
@@ -3571,9 +3510,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{0000000F-CF2F-4B92-BF82-37AF6163439F}"/>
                 </c:ext>
@@ -3595,9 +3532,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000010-CF2F-4B92-BF82-37AF6163439F}"/>
                 </c:ext>
@@ -3619,9 +3554,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000011-CF2F-4B92-BF82-37AF6163439F}"/>
                 </c:ext>
@@ -3653,9 +3586,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000013-CF2F-4B92-BF82-37AF6163439F}"/>
                 </c:ext>
@@ -3677,9 +3608,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000014-CF2F-4B92-BF82-37AF6163439F}"/>
                 </c:ext>
@@ -3701,9 +3630,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000015-CF2F-4B92-BF82-37AF6163439F}"/>
                 </c:ext>
@@ -3725,9 +3652,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000016-CF2F-4B92-BF82-37AF6163439F}"/>
                 </c:ext>
@@ -3749,9 +3674,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000017-CF2F-4B92-BF82-37AF6163439F}"/>
                 </c:ext>
@@ -3773,9 +3696,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000018-CF2F-4B92-BF82-37AF6163439F}"/>
                 </c:ext>
@@ -3820,7 +3741,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -4075,7 +3995,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4207,7 +4126,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4406,7 +4324,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4521,9 +4438,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000005-93BC-4033-9F9A-FD1B17CF6453}"/>
                 </c:ext>
@@ -4578,7 +4493,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -4741,9 +4655,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000007-93BC-4033-9F9A-FD1B17CF6453}"/>
                 </c:ext>
@@ -4775,9 +4687,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000003-93BC-4033-9F9A-FD1B17CF6453}"/>
                 </c:ext>
@@ -4809,9 +4719,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{0000000A-93BC-4033-9F9A-FD1B17CF6453}"/>
                 </c:ext>
@@ -4856,7 +4764,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -5154,9 +5061,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{0000000B-93BC-4033-9F9A-FD1B17CF6453}"/>
                 </c:ext>
@@ -5201,7 +5106,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -5387,7 +5291,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -5519,7 +5422,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -5718,7 +5620,7 @@
             </a:br>
             <a:r>
               <a:rPr lang="hu-HU" baseline="0"/>
-              <a:t>for 100 to 15000 points</a:t>
+              <a:t>for 100 to 10000 points</a:t>
             </a:r>
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
@@ -5774,7 +5676,7 @@
           <c:idx val="1"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Brute force</c:v>
+            <c:v>Naive</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -6070,7 +5972,7 @@
           <c:idx val="2"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Octree</c:v>
+            <c:v>Octree (Create+Search)</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -6221,7 +6123,7 @@
           <c:idx val="0"/>
           <c:order val="2"/>
           <c:tx>
-            <c:v>Octree (par)</c:v>
+            <c:v>Octree (Par. Create+Search)</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -6468,9 +6370,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000009-9AED-465E-B34D-BBC1C48444ED}"/>
                 </c:ext>
@@ -6492,9 +6392,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{0000000A-9AED-465E-B34D-BBC1C48444ED}"/>
                 </c:ext>
@@ -6694,7 +6592,7 @@
         <c:axId val="373844184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="15000"/>
+          <c:max val="10000"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -6814,16 +6712,17 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="426270320"/>
-        <c:crossesAt val="1.0000000000000002E-2"/>
+        <c:crossesAt val="1.0000000000000002E-3"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="3000"/>
+        <c:majorUnit val="1000"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="426270320"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
-          <c:min val="1.0000000000000002E-2"/>
+          <c:max val="100"/>
+          <c:min val="1.0000000000000002E-3"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -6971,7 +6870,7 @@
           <c:x val="0.79791055555555557"/>
           <c:y val="0.37863717948717951"/>
           <c:w val="0.19327"/>
-          <c:h val="0.34362008547008549"/>
+          <c:h val="0.24592777777777777"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -9660,8 +9559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M237"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S192" sqref="S192"/>
+    <sheetView tabSelected="1" topLeftCell="A184" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V230" sqref="V230"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update: Collision detection benchmark
</commit_message>
<xml_diff>
--- a/docs/report.xlsx
+++ b/docs/report.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="757" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="759" uniqueCount="23">
   <si>
     <t>Diagonally placed points</t>
   </si>
@@ -82,6 +82,12 @@
   </si>
   <si>
     <t>Box self conflict by octree</t>
+  </si>
+  <si>
+    <t>Create</t>
+  </si>
+  <si>
+    <t>Detection</t>
   </si>
 </sst>
 </file>
@@ -5717,7 +5723,18 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="hu-HU" baseline="0"/>
-              <a:t>Collision detection for 100 to 10000 points using OctreeBox</a:t>
+              <a:t>Collision detection using OctreeBox</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="hu-HU" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>for 100 to 10 000 boxes </a:t>
             </a:r>
             <a:endParaRPr lang="hu-HU"/>
           </a:p>
@@ -5761,9 +5778,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.11581555555555556"/>
-          <c:y val="9.8180769230769224E-2"/>
-          <c:w val="0.68839222222222218"/>
-          <c:h val="0.7813230769230769"/>
+          <c:y val="0.12260384615384616"/>
+          <c:w val="0.69015611111111108"/>
+          <c:h val="0.75690000000000002"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -5804,7 +5821,18 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
-              <c:delete val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.5875E-2"/>
+                  <c:y val="5.4273504273503279E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout/>
@@ -5815,10 +5843,47 @@
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-8.0684722222222227E-2"/>
+                  <c:y val="-3.1186965811965811E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-8C5D-4FE1-B287-AC51BF45D6BB}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
               <c:idx val="2"/>
-              <c:delete val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.9986111111111144E-2"/>
+                  <c:y val="-2.7136752136752137E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000002-9AED-465E-B34D-BBC1C48444ED}"/>
                 </c:ext>
@@ -5868,8 +5933,8 @@
               <c:idx val="11"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-4.9042500000000003E-2"/>
-                  <c:y val="-4.4673717948717946E-2"/>
+                  <c:x val="-3.669527777777791E-2"/>
+                  <c:y val="-3.6532692307692308E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:dLblPos val="r"/>
@@ -6004,46 +6069,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>3.6999999999999998E-2</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.28799999999999998</c:v>
+                  <c:v>0.214</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.86499999999999999</c:v>
+                  <c:v>0.63200000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.5389999999999999</c:v>
+                  <c:v>0.99399999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.403</c:v>
+                  <c:v>1.403</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.391</c:v>
+                  <c:v>1.8560000000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.5999999999999996</c:v>
+                  <c:v>2.4020000000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6.633</c:v>
+                  <c:v>3.585</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8.6769999999999996</c:v>
+                  <c:v>4.923</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10.805999999999999</c:v>
+                  <c:v>6.5149999999999997</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>13.497</c:v>
+                  <c:v>8.4410000000000007</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>16.407</c:v>
+                  <c:v>10.307</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>23.131</c:v>
+                  <c:v>14.882</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6090,8 +6155,8 @@
               <c:idx val="0"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="2.1620833333333332E-2"/>
-                  <c:y val="3.3900641025640929E-2"/>
+                  <c:x val="-8.4212499999999996E-2"/>
+                  <c:y val="3.1186965811965811E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:dLblPos val="r"/>
@@ -6298,46 +6363,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>5.8999999999999997E-2</c:v>
+                  <c:v>3.7999999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.254</c:v>
+                  <c:v>0.14499999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.5</c:v>
+                  <c:v>0.28599999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.75700000000000001</c:v>
+                  <c:v>0.39100000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.0309999999999999</c:v>
+                  <c:v>0.47699999999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.369</c:v>
+                  <c:v>0.56000000000000005</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.6830000000000001</c:v>
+                  <c:v>0.65400000000000003</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.9870000000000001</c:v>
+                  <c:v>0.75900000000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.262</c:v>
+                  <c:v>0.85799999999999998</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.8130000000000002</c:v>
+                  <c:v>1.0629999999999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.3159999999999998</c:v>
+                  <c:v>1.2949999999999999</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.9239999999999999</c:v>
+                  <c:v>1.587</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4.4770000000000003</c:v>
+                  <c:v>1.825</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6.1219999999999999</c:v>
+                  <c:v>2.5310000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6382,7 +6447,18 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
-              <c:delete val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.0583333333333318E-2"/>
+                  <c:y val="4.3418803418803421E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout/>
@@ -6394,7 +6470,18 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
-              <c:delete val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-6.8791666666666668E-2"/>
+                  <c:y val="-6.2414529914529913E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout/>
@@ -6428,8 +6515,8 @@
               <c:idx val="4"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-2.7729861111111143E-2"/>
-                  <c:y val="-3.6310897435897535E-2"/>
+                  <c:x val="-7.8882638888888884E-2"/>
+                  <c:y val="-3.6310897435897486E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:dLblPos val="r"/>
@@ -6462,9 +6549,7 @@
               <c:idx val="6"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{0000000B-DBE6-43DE-910A-83DED8CCA67B}"/>
                 </c:ext>
@@ -6474,8 +6559,8 @@
               <c:idx val="7"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-5.9367361111111114E-2"/>
-                  <c:y val="3.9017307692307594E-2"/>
+                  <c:x val="-8.0534027777777781E-2"/>
+                  <c:y val="-3.9679273504273506E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:dLblPos val="r"/>
@@ -6498,8 +6583,8 @@
               <c:idx val="8"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-1.7184722222222223E-2"/>
-                  <c:y val="-2.0372863247863249E-2"/>
+                  <c:x val="-4.011527777777784E-2"/>
+                  <c:y val="-4.7509615384615386E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:dLblPos val="r"/>
@@ -6515,6 +6600,54 @@
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000006-9AED-465E-B34D-BBC1C48444ED}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="9"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.1192500000000002E-2"/>
+                  <c:y val="-3.9368589743589741E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-8C5D-4FE1-B287-AC51BF45D6BB}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="10"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.345027777777784E-2"/>
+                  <c:y val="-4.4795940170940199E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-8C5D-4FE1-B287-AC51BF45D6BB}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -6606,9 +6739,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000009-9AED-465E-B34D-BBC1C48444ED}"/>
                 </c:ext>
@@ -6630,9 +6761,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{0000000A-9AED-465E-B34D-BBC1C48444ED}"/>
                 </c:ext>
@@ -6677,7 +6806,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -6870,7 +6998,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="hu-HU"/>
-                  <a:t>Number of points</a:t>
+                  <a:t>Number of boxes</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -6905,7 +7033,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.0E+00" sourceLinked="0"/>
+        <c:numFmt formatCode="#,##0" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -7098,7 +7226,1160 @@
           <c:x val="0.79791055555555557"/>
           <c:y val="0.37863717948717951"/>
           <c:w val="0.19327"/>
-          <c:h val="0.24592777777777777"/>
+          <c:h val="0.20522264957264955"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="hu-HU"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="hu-HU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="hu-HU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="hu-HU" baseline="0"/>
+              <a:t>Using Morton Z-order (OctreeBox) vs. typical implementation performace for 10 to 100M box</a:t>
+            </a:r>
+            <a:endParaRPr lang="hu-HU"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="hu-HU"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.11581555555555556"/>
+          <c:y val="0.14702692307692308"/>
+          <c:w val="0.66369777777777794"/>
+          <c:h val="0.73247692307692303"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Typical</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-6.8337499999999995E-2"/>
+                  <c:y val="1.3771367521367521E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-4843-443B-A16F-AD756CF3E9EF}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000006-4843-443B-A16F-AD756CF3E9EF}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.1295833333333335E-2"/>
+                  <c:y val="-6.6464743589743594E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000007-4843-443B-A16F-AD756CF3E9EF}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000008-4843-443B-A16F-AD756CF3E9EF}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="10"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.5811388888888886E-2"/>
+                  <c:y val="-2.5759615384615384E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000009-4843-443B-A16F-AD756CF3E9EF}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="hu-HU"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>report!$D$213:$D$224</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7500</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10000000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>100000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>report!$E$213:$E$224</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>4.0000000000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.112</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.25800000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.39100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.55500000000000005</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.5860000000000003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>76.27</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>819.03399999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8992.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-4843-443B-A16F-AD756CF3E9EF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Morton (unseq)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="dash"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>report!$D$189:$D$200</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7500</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10000000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>100000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>report!$E$189:$E$200</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>8.9999999999999998E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.1999999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.22900000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.44500000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.69499999999999995</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.85299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.8849999999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>84.283000000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>785.20600000000002</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7903.49</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000B-4843-443B-A16F-AD756CF3E9EF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Morton (par)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+                <a:prstDash val="dash"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000C-4843-443B-A16F-AD756CF3E9EF}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.355361111111111E-2"/>
+                  <c:y val="-5.8323717948717949E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000D-4843-443B-A16F-AD756CF3E9EF}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="9"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.0598671251488763E-2"/>
+                  <c:y val="4.1793789575924931E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000011-4843-443B-A16F-AD756CF3E9EF}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="10"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.1091426461204318E-2"/>
+                  <c:y val="3.9098716699668933E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000010-4843-443B-A16F-AD756CF3E9EF}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="11"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.5306174059264909E-2"/>
+                  <c:y val="3.370857094715686E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000F-4843-443B-A16F-AD756CF3E9EF}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="hu-HU"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>report!$D$201:$D$212</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7500</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10000000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>100000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>report!$E$201:$E$212</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.127</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.223</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.34300000000000003</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.35299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.5470000000000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>29.695</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>250.864</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2730.17</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000E-4843-443B-A16F-AD756CF3E9EF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="373844184"/>
+        <c:axId val="426270320"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="373844184"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:max val="100000000"/>
+          <c:min val="10"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="bg2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="hu-HU"/>
+                  <a:t>Number of points (log</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="hu-HU" baseline="0"/>
+                  <a:t> scale)</a:t>
+                </a:r>
+                <a:endParaRPr lang="hu-HU"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="hu-HU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.0E+00" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="hu-HU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="426270320"/>
+        <c:crossesAt val="1.0000000000000003E-4"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="10"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="426270320"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="bg2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="hu-HU"/>
+                  <a:t>Time </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="hu-HU" baseline="0"/>
+                  <a:t>[ms]</a:t>
+                </a:r>
+                <a:endParaRPr lang="hu-HU"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="hu-HU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="in"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="hu-HU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="373844184"/>
+        <c:crossesAt val="1.0000000000000003E-4"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.80929680555555561"/>
+          <c:y val="0.46157371794871804"/>
+          <c:w val="0.13425875000000001"/>
+          <c:h val="0.18317435897435899"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -7288,6 +8569,46 @@
 </file>
 
 <file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -9391,6 +10712,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -9489,16 +11326,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>194</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>429986</xdr:colOff>
+      <xdr:row>241</xdr:row>
+      <xdr:rowOff>25852</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>418200</xdr:colOff>
-      <xdr:row>220</xdr:row>
-      <xdr:rowOff>41325</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>91629</xdr:colOff>
+      <xdr:row>267</xdr:row>
+      <xdr:rowOff>503</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9514,6 +11351,38 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>81644</xdr:colOff>
+      <xdr:row>190</xdr:row>
+      <xdr:rowOff>40820</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>423644</xdr:colOff>
+      <xdr:row>216</xdr:row>
+      <xdr:rowOff>15470</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Diagram 7"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -9787,8 +11656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M267"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" topLeftCell="E229" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="P272" sqref="P272"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -14660,7 +16529,7 @@
         <v>10</v>
       </c>
       <c r="E189">
-        <v>0</v>
+        <v>8.9999999999999998E-4</v>
       </c>
       <c r="F189" t="s">
         <v>2</v>
@@ -15140,7 +17009,7 @@
         <v>10</v>
       </c>
       <c r="E213">
-        <v>0</v>
+        <v>4.0000000000000002E-4</v>
       </c>
       <c r="F213">
         <v>1080</v>
@@ -15366,7 +17235,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="225" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>18</v>
       </c>
@@ -15386,7 +17255,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="226" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>19</v>
       </c>
@@ -15406,7 +17275,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="227" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>19</v>
       </c>
@@ -15426,7 +17295,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="228" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>19</v>
       </c>
@@ -15446,7 +17315,7 @@
         <v>1524</v>
       </c>
     </row>
-    <row r="229" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>19</v>
       </c>
@@ -15466,7 +17335,7 @@
         <v>2762</v>
       </c>
     </row>
-    <row r="230" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>19</v>
       </c>
@@ -15486,7 +17355,7 @@
         <v>4179</v>
       </c>
     </row>
-    <row r="231" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>19</v>
       </c>
@@ -15506,7 +17375,7 @@
         <v>5980</v>
       </c>
     </row>
-    <row r="232" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>19</v>
       </c>
@@ -15526,7 +17395,7 @@
         <v>8075</v>
       </c>
     </row>
-    <row r="233" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>19</v>
       </c>
@@ -15546,7 +17415,7 @@
         <v>10554</v>
       </c>
     </row>
-    <row r="234" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>19</v>
       </c>
@@ -15566,7 +17435,7 @@
         <v>13285</v>
       </c>
     </row>
-    <row r="235" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>19</v>
       </c>
@@ -15586,7 +17455,7 @@
         <v>19374</v>
       </c>
     </row>
-    <row r="236" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>19</v>
       </c>
@@ -15606,7 +17475,7 @@
         <v>26769</v>
       </c>
     </row>
-    <row r="237" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>19</v>
       </c>
@@ -15626,7 +17495,7 @@
         <v>35258</v>
       </c>
     </row>
-    <row r="238" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>19</v>
       </c>
@@ -15646,7 +17515,7 @@
         <v>44931</v>
       </c>
     </row>
-    <row r="239" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>19</v>
       </c>
@@ -15665,8 +17534,14 @@
       <c r="F239">
         <v>67944</v>
       </c>
-    </row>
-    <row r="240" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H239" t="s">
+        <v>21</v>
+      </c>
+      <c r="I239" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="240" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>20</v>
       </c>
@@ -15680,13 +17555,20 @@
         <v>100</v>
       </c>
       <c r="E240">
-        <v>3.6999999999999998E-2</v>
+        <v>0.03</v>
       </c>
       <c r="F240">
         <v>105</v>
       </c>
-    </row>
-    <row r="241" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H240">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="I240">
+        <f>E240-H240</f>
+        <v>1.2999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="241" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>20</v>
       </c>
@@ -15700,13 +17582,20 @@
         <v>500</v>
       </c>
       <c r="E241">
-        <v>0.28799999999999998</v>
+        <v>0.214</v>
       </c>
       <c r="F241">
         <v>617</v>
       </c>
-    </row>
-    <row r="242" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H241">
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="I241">
+        <f t="shared" ref="I241:I267" si="0">E241-H241</f>
+        <v>0.11499999999999999</v>
+      </c>
+    </row>
+    <row r="242" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>20</v>
       </c>
@@ -15720,13 +17609,20 @@
         <v>1000</v>
       </c>
       <c r="E242">
-        <v>0.86499999999999999</v>
+        <v>0.63200000000000001</v>
       </c>
       <c r="F242">
         <v>1524</v>
       </c>
-    </row>
-    <row r="243" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H242">
+        <v>0.33100000000000002</v>
+      </c>
+      <c r="I242">
+        <f t="shared" si="0"/>
+        <v>0.30099999999999999</v>
+      </c>
+    </row>
+    <row r="243" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>20</v>
       </c>
@@ -15740,13 +17636,20 @@
         <v>1500</v>
       </c>
       <c r="E243">
-        <v>1.5389999999999999</v>
+        <v>0.99399999999999999</v>
       </c>
       <c r="F243">
         <v>2762</v>
       </c>
-    </row>
-    <row r="244" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H243">
+        <v>0.55900000000000005</v>
+      </c>
+      <c r="I243">
+        <f t="shared" si="0"/>
+        <v>0.43499999999999994</v>
+      </c>
+    </row>
+    <row r="244" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>20</v>
       </c>
@@ -15760,13 +17663,20 @@
         <v>2000</v>
       </c>
       <c r="E244">
-        <v>2.403</v>
+        <v>1.403</v>
       </c>
       <c r="F244">
         <v>4180</v>
       </c>
-    </row>
-    <row r="245" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H244">
+        <v>0.76</v>
+      </c>
+      <c r="I244">
+        <f t="shared" si="0"/>
+        <v>0.64300000000000002</v>
+      </c>
+    </row>
+    <row r="245" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>20</v>
       </c>
@@ -15780,13 +17690,20 @@
         <v>2500</v>
       </c>
       <c r="E245">
-        <v>3.391</v>
+        <v>1.8560000000000001</v>
       </c>
       <c r="F245">
         <v>5981</v>
       </c>
-    </row>
-    <row r="246" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H245">
+        <v>1</v>
+      </c>
+      <c r="I245">
+        <f t="shared" si="0"/>
+        <v>0.85600000000000009</v>
+      </c>
+    </row>
+    <row r="246" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>20</v>
       </c>
@@ -15800,13 +17717,20 @@
         <v>3000</v>
       </c>
       <c r="E246">
-        <v>4.5999999999999996</v>
+        <v>2.4020000000000001</v>
       </c>
       <c r="F246">
         <v>8077</v>
       </c>
-    </row>
-    <row r="247" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H246">
+        <v>1.2410000000000001</v>
+      </c>
+      <c r="I246">
+        <f t="shared" si="0"/>
+        <v>1.161</v>
+      </c>
+    </row>
+    <row r="247" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>20</v>
       </c>
@@ -15820,13 +17744,20 @@
         <v>3500</v>
       </c>
       <c r="E247">
-        <v>5.5</v>
+        <v>3</v>
       </c>
       <c r="F247">
         <v>10556</v>
       </c>
-    </row>
-    <row r="248" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H247">
+        <v>1.454</v>
+      </c>
+      <c r="I247">
+        <f t="shared" si="0"/>
+        <v>1.546</v>
+      </c>
+    </row>
+    <row r="248" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>20</v>
       </c>
@@ -15840,13 +17771,20 @@
         <v>4000</v>
       </c>
       <c r="E248">
-        <v>6.633</v>
+        <v>3.585</v>
       </c>
       <c r="F248">
         <v>13288</v>
       </c>
-    </row>
-    <row r="249" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H248">
+        <v>1.639</v>
+      </c>
+      <c r="I248">
+        <f t="shared" si="0"/>
+        <v>1.946</v>
+      </c>
+    </row>
+    <row r="249" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>20</v>
       </c>
@@ -15860,13 +17798,20 @@
         <v>5000</v>
       </c>
       <c r="E249">
-        <v>8.6769999999999996</v>
+        <v>4.923</v>
       </c>
       <c r="F249">
         <v>19380</v>
       </c>
-    </row>
-    <row r="250" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H249">
+        <v>2.0409999999999999</v>
+      </c>
+      <c r="I249">
+        <f t="shared" si="0"/>
+        <v>2.8820000000000001</v>
+      </c>
+    </row>
+    <row r="250" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>20</v>
       </c>
@@ -15880,13 +17825,20 @@
         <v>6000</v>
       </c>
       <c r="E250">
-        <v>10.805999999999999</v>
+        <v>6.5149999999999997</v>
       </c>
       <c r="F250">
         <v>26785</v>
       </c>
-    </row>
-    <row r="251" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H250">
+        <v>2.3620000000000001</v>
+      </c>
+      <c r="I250">
+        <f t="shared" si="0"/>
+        <v>4.1529999999999996</v>
+      </c>
+    </row>
+    <row r="251" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>20</v>
       </c>
@@ -15900,13 +17852,20 @@
         <v>7000</v>
       </c>
       <c r="E251">
-        <v>13.497</v>
+        <v>8.4410000000000007</v>
       </c>
       <c r="F251">
         <v>35282</v>
       </c>
-    </row>
-    <row r="252" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H251">
+        <v>2.6890000000000001</v>
+      </c>
+      <c r="I251">
+        <f t="shared" si="0"/>
+        <v>5.7520000000000007</v>
+      </c>
+    </row>
+    <row r="252" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
         <v>20</v>
       </c>
@@ -15920,13 +17879,20 @@
         <v>8000</v>
       </c>
       <c r="E252">
-        <v>16.407</v>
+        <v>10.307</v>
       </c>
       <c r="F252">
         <v>44957</v>
       </c>
-    </row>
-    <row r="253" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H252">
+        <v>3.048</v>
+      </c>
+      <c r="I252">
+        <f t="shared" si="0"/>
+        <v>7.2590000000000003</v>
+      </c>
+    </row>
+    <row r="253" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>20</v>
       </c>
@@ -15940,13 +17906,20 @@
         <v>10000</v>
       </c>
       <c r="E253">
-        <v>23.131</v>
+        <v>14.882</v>
       </c>
       <c r="F253">
         <v>67994</v>
       </c>
-    </row>
-    <row r="254" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H253">
+        <v>3.7330000000000001</v>
+      </c>
+      <c r="I253">
+        <f t="shared" si="0"/>
+        <v>11.148999999999999</v>
+      </c>
+    </row>
+    <row r="254" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
         <v>20</v>
       </c>
@@ -15960,13 +17933,20 @@
         <v>100</v>
       </c>
       <c r="E254">
-        <v>5.8999999999999997E-2</v>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="F254">
         <v>105</v>
       </c>
-    </row>
-    <row r="255" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H254">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="I254">
+        <f t="shared" si="0"/>
+        <v>9.9999999999999985E-3</v>
+      </c>
+    </row>
+    <row r="255" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>20</v>
       </c>
@@ -15980,13 +17960,20 @@
         <v>500</v>
       </c>
       <c r="E255">
-        <v>0.254</v>
+        <v>0.14499999999999999</v>
       </c>
       <c r="F255">
         <v>617</v>
       </c>
-    </row>
-    <row r="256" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H255">
+        <v>0.127</v>
+      </c>
+      <c r="I255">
+        <f t="shared" si="0"/>
+        <v>1.7999999999999988E-2</v>
+      </c>
+    </row>
+    <row r="256" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>20</v>
       </c>
@@ -16000,13 +17987,20 @@
         <v>1000</v>
       </c>
       <c r="E256">
-        <v>0.5</v>
+        <v>0.28599999999999998</v>
       </c>
       <c r="F256">
         <v>1524</v>
       </c>
-    </row>
-    <row r="257" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H256">
+        <v>0.26700000000000002</v>
+      </c>
+      <c r="I256">
+        <f t="shared" si="0"/>
+        <v>1.8999999999999961E-2</v>
+      </c>
+    </row>
+    <row r="257" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>20</v>
       </c>
@@ -16020,13 +18014,20 @@
         <v>1500</v>
       </c>
       <c r="E257">
-        <v>0.75700000000000001</v>
+        <v>0.39100000000000001</v>
       </c>
       <c r="F257">
         <v>2762</v>
       </c>
-    </row>
-    <row r="258" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H257">
+        <v>0.38200000000000001</v>
+      </c>
+      <c r="I257">
+        <f t="shared" si="0"/>
+        <v>9.000000000000008E-3</v>
+      </c>
+    </row>
+    <row r="258" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
         <v>20</v>
       </c>
@@ -16040,13 +18041,20 @@
         <v>2000</v>
       </c>
       <c r="E258">
-        <v>1.0309999999999999</v>
+        <v>0.47699999999999998</v>
       </c>
       <c r="F258">
         <v>4180</v>
       </c>
-    </row>
-    <row r="259" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H258">
+        <v>0.51</v>
+      </c>
+      <c r="I258">
+        <f t="shared" si="0"/>
+        <v>-3.3000000000000029E-2</v>
+      </c>
+    </row>
+    <row r="259" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
         <v>20</v>
       </c>
@@ -16060,13 +18068,20 @@
         <v>2500</v>
       </c>
       <c r="E259">
-        <v>1.369</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="F259">
         <v>5981</v>
       </c>
-    </row>
-    <row r="260" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H259">
+        <v>0.65100000000000002</v>
+      </c>
+      <c r="I259">
+        <f t="shared" si="0"/>
+        <v>-9.099999999999997E-2</v>
+      </c>
+    </row>
+    <row r="260" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
         <v>20</v>
       </c>
@@ -16080,13 +18095,20 @@
         <v>3000</v>
       </c>
       <c r="E260">
-        <v>1.6830000000000001</v>
+        <v>0.65400000000000003</v>
       </c>
       <c r="F260">
         <v>8077</v>
       </c>
-    </row>
-    <row r="261" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H260">
+        <v>0.79</v>
+      </c>
+      <c r="I260">
+        <f t="shared" si="0"/>
+        <v>-0.13600000000000001</v>
+      </c>
+    </row>
+    <row r="261" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
         <v>20</v>
       </c>
@@ -16100,13 +18122,20 @@
         <v>3500</v>
       </c>
       <c r="E261">
-        <v>1.9870000000000001</v>
+        <v>0.75900000000000001</v>
       </c>
       <c r="F261">
         <v>10556</v>
       </c>
-    </row>
-    <row r="262" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H261">
+        <v>0.92300000000000004</v>
+      </c>
+      <c r="I261">
+        <f t="shared" si="0"/>
+        <v>-0.16400000000000003</v>
+      </c>
+    </row>
+    <row r="262" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
         <v>20</v>
       </c>
@@ -16120,13 +18149,20 @@
         <v>4000</v>
       </c>
       <c r="E262">
-        <v>2.262</v>
+        <v>0.85799999999999998</v>
       </c>
       <c r="F262">
         <v>13288</v>
       </c>
-    </row>
-    <row r="263" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H262">
+        <v>1.01</v>
+      </c>
+      <c r="I262">
+        <f t="shared" si="0"/>
+        <v>-0.15200000000000002</v>
+      </c>
+    </row>
+    <row r="263" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
         <v>20</v>
       </c>
@@ -16140,13 +18176,20 @@
         <v>5000</v>
       </c>
       <c r="E263">
-        <v>2.8130000000000002</v>
+        <v>1.0629999999999999</v>
       </c>
       <c r="F263">
         <v>19380</v>
       </c>
-    </row>
-    <row r="264" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H263">
+        <v>1.1919999999999999</v>
+      </c>
+      <c r="I263">
+        <f t="shared" si="0"/>
+        <v>-0.129</v>
+      </c>
+    </row>
+    <row r="264" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
         <v>20</v>
       </c>
@@ -16160,13 +18203,20 @@
         <v>6000</v>
       </c>
       <c r="E264">
-        <v>3.3159999999999998</v>
+        <v>1.2949999999999999</v>
       </c>
       <c r="F264">
         <v>26785</v>
       </c>
-    </row>
-    <row r="265" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H264">
+        <v>1.3620000000000001</v>
+      </c>
+      <c r="I264">
+        <f t="shared" si="0"/>
+        <v>-6.7000000000000171E-2</v>
+      </c>
+    </row>
+    <row r="265" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
         <v>20</v>
       </c>
@@ -16180,13 +18230,20 @@
         <v>7000</v>
       </c>
       <c r="E265">
-        <v>3.9239999999999999</v>
+        <v>1.587</v>
       </c>
       <c r="F265">
         <v>35282</v>
       </c>
-    </row>
-    <row r="266" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H265">
+        <v>1.5269999999999999</v>
+      </c>
+      <c r="I265">
+        <f t="shared" si="0"/>
+        <v>6.0000000000000053E-2</v>
+      </c>
+    </row>
+    <row r="266" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
         <v>20</v>
       </c>
@@ -16200,13 +18257,20 @@
         <v>8000</v>
       </c>
       <c r="E266">
-        <v>4.4770000000000003</v>
+        <v>1.825</v>
       </c>
       <c r="F266">
         <v>44957</v>
       </c>
-    </row>
-    <row r="267" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H266">
+        <v>1.679</v>
+      </c>
+      <c r="I266">
+        <f t="shared" si="0"/>
+        <v>0.14599999999999991</v>
+      </c>
+    </row>
+    <row r="267" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
         <v>20</v>
       </c>
@@ -16220,10 +18284,17 @@
         <v>10000</v>
       </c>
       <c r="E267">
-        <v>6.1219999999999999</v>
+        <v>2.5310000000000001</v>
       </c>
       <c r="F267">
         <v>67994</v>
+      </c>
+      <c r="H267">
+        <v>2.06</v>
+      </c>
+      <c r="I267">
+        <f t="shared" si="0"/>
+        <v>0.47100000000000009</v>
       </c>
     </row>
   </sheetData>

</xml_diff>